<commit_message>
Cleaning relevance assessment dataset
</commit_message>
<xml_diff>
--- a/data/search_session_stats.xlsx
+++ b/data/search_session_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C345"/>
+  <dimension ref="A1:D345"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>num_results</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>num_unique_urls</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -462,6 +467,9 @@
       <c r="C2" t="n">
         <v>10</v>
       </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -475,6 +483,9 @@
       <c r="C3" t="n">
         <v>12</v>
       </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -488,6 +499,9 @@
       <c r="C4" t="n">
         <v>10</v>
       </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -501,6 +515,9 @@
       <c r="C5" t="n">
         <v>10</v>
       </c>
+      <c r="D5" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -514,6 +531,9 @@
       <c r="C6" t="n">
         <v>13</v>
       </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -527,6 +547,9 @@
       <c r="C7" t="n">
         <v>10</v>
       </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -540,6 +563,9 @@
       <c r="C8" t="n">
         <v>10</v>
       </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -553,6 +579,9 @@
       <c r="C9" t="n">
         <v>10</v>
       </c>
+      <c r="D9" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -566,6 +595,9 @@
       <c r="C10" t="n">
         <v>12</v>
       </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -579,6 +611,9 @@
       <c r="C11" t="n">
         <v>6</v>
       </c>
+      <c r="D11" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -592,6 +627,9 @@
       <c r="C12" t="n">
         <v>10</v>
       </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -605,6 +643,9 @@
       <c r="C13" t="n">
         <v>10</v>
       </c>
+      <c r="D13" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -618,6 +659,9 @@
       <c r="C14" t="n">
         <v>10</v>
       </c>
+      <c r="D14" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -631,6 +675,9 @@
       <c r="C15" t="n">
         <v>10</v>
       </c>
+      <c r="D15" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -644,6 +691,9 @@
       <c r="C16" t="n">
         <v>10</v>
       </c>
+      <c r="D16" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -657,6 +707,9 @@
       <c r="C17" t="n">
         <v>10</v>
       </c>
+      <c r="D17" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -670,6 +723,9 @@
       <c r="C18" t="n">
         <v>10</v>
       </c>
+      <c r="D18" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -683,6 +739,9 @@
       <c r="C19" t="n">
         <v>10</v>
       </c>
+      <c r="D19" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -696,6 +755,9 @@
       <c r="C20" t="n">
         <v>10</v>
       </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -709,6 +771,9 @@
       <c r="C21" t="n">
         <v>10</v>
       </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -722,6 +787,9 @@
       <c r="C22" t="n">
         <v>10</v>
       </c>
+      <c r="D22" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -735,6 +803,9 @@
       <c r="C23" t="n">
         <v>10</v>
       </c>
+      <c r="D23" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -748,6 +819,9 @@
       <c r="C24" t="n">
         <v>10</v>
       </c>
+      <c r="D24" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -761,6 +835,9 @@
       <c r="C25" t="n">
         <v>10</v>
       </c>
+      <c r="D25" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -774,6 +851,9 @@
       <c r="C26" t="n">
         <v>10</v>
       </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -787,6 +867,9 @@
       <c r="C27" t="n">
         <v>10</v>
       </c>
+      <c r="D27" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -800,6 +883,9 @@
       <c r="C28" t="n">
         <v>10</v>
       </c>
+      <c r="D28" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -813,6 +899,9 @@
       <c r="C29" t="n">
         <v>9</v>
       </c>
+      <c r="D29" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -826,6 +915,9 @@
       <c r="C30" t="n">
         <v>10</v>
       </c>
+      <c r="D30" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -839,6 +931,9 @@
       <c r="C31" t="n">
         <v>10</v>
       </c>
+      <c r="D31" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -852,6 +947,9 @@
       <c r="C32" t="n">
         <v>10</v>
       </c>
+      <c r="D32" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -865,6 +963,9 @@
       <c r="C33" t="n">
         <v>10</v>
       </c>
+      <c r="D33" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -878,6 +979,9 @@
       <c r="C34" t="n">
         <v>10</v>
       </c>
+      <c r="D34" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -891,6 +995,9 @@
       <c r="C35" t="n">
         <v>9</v>
       </c>
+      <c r="D35" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -904,6 +1011,9 @@
       <c r="C36" t="n">
         <v>10</v>
       </c>
+      <c r="D36" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -917,6 +1027,9 @@
       <c r="C37" t="n">
         <v>10</v>
       </c>
+      <c r="D37" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -930,6 +1043,9 @@
       <c r="C38" t="n">
         <v>10</v>
       </c>
+      <c r="D38" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -943,6 +1059,9 @@
       <c r="C39" t="n">
         <v>10</v>
       </c>
+      <c r="D39" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -956,6 +1075,9 @@
       <c r="C40" t="n">
         <v>10</v>
       </c>
+      <c r="D40" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -969,6 +1091,9 @@
       <c r="C41" t="n">
         <v>12</v>
       </c>
+      <c r="D41" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -982,6 +1107,9 @@
       <c r="C42" t="n">
         <v>10</v>
       </c>
+      <c r="D42" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -995,6 +1123,9 @@
       <c r="C43" t="n">
         <v>10</v>
       </c>
+      <c r="D43" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1008,6 +1139,9 @@
       <c r="C44" t="n">
         <v>10</v>
       </c>
+      <c r="D44" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1021,6 +1155,9 @@
       <c r="C45" t="n">
         <v>10</v>
       </c>
+      <c r="D45" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1034,6 +1171,9 @@
       <c r="C46" t="n">
         <v>10</v>
       </c>
+      <c r="D46" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1047,6 +1187,9 @@
       <c r="C47" t="n">
         <v>10</v>
       </c>
+      <c r="D47" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1060,6 +1203,9 @@
       <c r="C48" t="n">
         <v>10</v>
       </c>
+      <c r="D48" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1073,6 +1219,9 @@
       <c r="C49" t="n">
         <v>19</v>
       </c>
+      <c r="D49" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1086,6 +1235,9 @@
       <c r="C50" t="n">
         <v>18</v>
       </c>
+      <c r="D50" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1099,6 +1251,9 @@
       <c r="C51" t="n">
         <v>19</v>
       </c>
+      <c r="D51" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1112,6 +1267,9 @@
       <c r="C52" t="n">
         <v>8</v>
       </c>
+      <c r="D52" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1125,6 +1283,9 @@
       <c r="C53" t="n">
         <v>16</v>
       </c>
+      <c r="D53" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1138,6 +1299,9 @@
       <c r="C54" t="n">
         <v>17</v>
       </c>
+      <c r="D54" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1151,6 +1315,9 @@
       <c r="C55" t="n">
         <v>16</v>
       </c>
+      <c r="D55" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1164,6 +1331,9 @@
       <c r="C56" t="n">
         <v>15</v>
       </c>
+      <c r="D56" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1177,6 +1347,9 @@
       <c r="C57" t="n">
         <v>10</v>
       </c>
+      <c r="D57" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1190,6 +1363,9 @@
       <c r="C58" t="n">
         <v>11</v>
       </c>
+      <c r="D58" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1203,6 +1379,9 @@
       <c r="C59" t="n">
         <v>18</v>
       </c>
+      <c r="D59" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1216,6 +1395,9 @@
       <c r="C60" t="n">
         <v>16</v>
       </c>
+      <c r="D60" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1229,6 +1411,9 @@
       <c r="C61" t="n">
         <v>15</v>
       </c>
+      <c r="D61" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1242,6 +1427,9 @@
       <c r="C62" t="n">
         <v>13</v>
       </c>
+      <c r="D62" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1255,6 +1443,9 @@
       <c r="C63" t="n">
         <v>15</v>
       </c>
+      <c r="D63" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -1268,6 +1459,9 @@
       <c r="C64" t="n">
         <v>19</v>
       </c>
+      <c r="D64" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -1281,6 +1475,9 @@
       <c r="C65" t="n">
         <v>10</v>
       </c>
+      <c r="D65" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1294,6 +1491,9 @@
       <c r="C66" t="n">
         <v>17</v>
       </c>
+      <c r="D66" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1307,6 +1507,9 @@
       <c r="C67" t="n">
         <v>19</v>
       </c>
+      <c r="D67" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -1320,6 +1523,9 @@
       <c r="C68" t="n">
         <v>10</v>
       </c>
+      <c r="D68" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -1333,6 +1539,9 @@
       <c r="C69" t="n">
         <v>10</v>
       </c>
+      <c r="D69" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -1346,6 +1555,9 @@
       <c r="C70" t="n">
         <v>10</v>
       </c>
+      <c r="D70" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -1359,6 +1571,9 @@
       <c r="C71" t="n">
         <v>10</v>
       </c>
+      <c r="D71" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -1372,6 +1587,9 @@
       <c r="C72" t="n">
         <v>10</v>
       </c>
+      <c r="D72" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -1385,6 +1603,9 @@
       <c r="C73" t="n">
         <v>10</v>
       </c>
+      <c r="D73" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -1398,6 +1619,9 @@
       <c r="C74" t="n">
         <v>10</v>
       </c>
+      <c r="D74" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -1411,6 +1635,9 @@
       <c r="C75" t="n">
         <v>10</v>
       </c>
+      <c r="D75" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -1424,6 +1651,9 @@
       <c r="C76" t="n">
         <v>10</v>
       </c>
+      <c r="D76" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -1437,6 +1667,9 @@
       <c r="C77" t="n">
         <v>10</v>
       </c>
+      <c r="D77" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1450,6 +1683,9 @@
       <c r="C78" t="n">
         <v>10</v>
       </c>
+      <c r="D78" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -1463,6 +1699,9 @@
       <c r="C79" t="n">
         <v>19</v>
       </c>
+      <c r="D79" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -1476,6 +1715,9 @@
       <c r="C80" t="n">
         <v>10</v>
       </c>
+      <c r="D80" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -1489,6 +1731,9 @@
       <c r="C81" t="n">
         <v>10</v>
       </c>
+      <c r="D81" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -1502,6 +1747,9 @@
       <c r="C82" t="n">
         <v>10</v>
       </c>
+      <c r="D82" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -1515,6 +1763,9 @@
       <c r="C83" t="n">
         <v>9</v>
       </c>
+      <c r="D83" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -1528,6 +1779,9 @@
       <c r="C84" t="n">
         <v>9</v>
       </c>
+      <c r="D84" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -1541,6 +1795,9 @@
       <c r="C85" t="n">
         <v>10</v>
       </c>
+      <c r="D85" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -1554,6 +1811,9 @@
       <c r="C86" t="n">
         <v>10</v>
       </c>
+      <c r="D86" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -1567,6 +1827,9 @@
       <c r="C87" t="n">
         <v>10</v>
       </c>
+      <c r="D87" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -1580,6 +1843,9 @@
       <c r="C88" t="n">
         <v>10</v>
       </c>
+      <c r="D88" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -1593,6 +1859,9 @@
       <c r="C89" t="n">
         <v>15</v>
       </c>
+      <c r="D89" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -1606,6 +1875,9 @@
       <c r="C90" t="n">
         <v>10</v>
       </c>
+      <c r="D90" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -1619,6 +1891,9 @@
       <c r="C91" t="n">
         <v>16</v>
       </c>
+      <c r="D91" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -1632,6 +1907,9 @@
       <c r="C92" t="n">
         <v>10</v>
       </c>
+      <c r="D92" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -1645,6 +1923,9 @@
       <c r="C93" t="n">
         <v>11</v>
       </c>
+      <c r="D93" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -1658,6 +1939,9 @@
       <c r="C94" t="n">
         <v>10</v>
       </c>
+      <c r="D94" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -1671,6 +1955,9 @@
       <c r="C95" t="n">
         <v>10</v>
       </c>
+      <c r="D95" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -1684,6 +1971,9 @@
       <c r="C96" t="n">
         <v>17</v>
       </c>
+      <c r="D96" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -1697,6 +1987,9 @@
       <c r="C97" t="n">
         <v>19</v>
       </c>
+      <c r="D97" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -1710,6 +2003,9 @@
       <c r="C98" t="n">
         <v>17</v>
       </c>
+      <c r="D98" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -1723,6 +2019,9 @@
       <c r="C99" t="n">
         <v>13</v>
       </c>
+      <c r="D99" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -1736,6 +2035,9 @@
       <c r="C100" t="n">
         <v>18</v>
       </c>
+      <c r="D100" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -1749,6 +2051,9 @@
       <c r="C101" t="n">
         <v>15</v>
       </c>
+      <c r="D101" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -1762,6 +2067,9 @@
       <c r="C102" t="n">
         <v>10</v>
       </c>
+      <c r="D102" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -1775,6 +2083,9 @@
       <c r="C103" t="n">
         <v>13</v>
       </c>
+      <c r="D103" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -1788,6 +2099,9 @@
       <c r="C104" t="n">
         <v>15</v>
       </c>
+      <c r="D104" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -1801,6 +2115,9 @@
       <c r="C105" t="n">
         <v>18</v>
       </c>
+      <c r="D105" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -1814,6 +2131,9 @@
       <c r="C106" t="n">
         <v>18</v>
       </c>
+      <c r="D106" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -1827,6 +2147,9 @@
       <c r="C107" t="n">
         <v>19</v>
       </c>
+      <c r="D107" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -1840,6 +2163,9 @@
       <c r="C108" t="n">
         <v>19</v>
       </c>
+      <c r="D108" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -1853,6 +2179,9 @@
       <c r="C109" t="n">
         <v>17</v>
       </c>
+      <c r="D109" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -1866,6 +2195,9 @@
       <c r="C110" t="n">
         <v>16</v>
       </c>
+      <c r="D110" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -1879,6 +2211,9 @@
       <c r="C111" t="n">
         <v>17</v>
       </c>
+      <c r="D111" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -1892,6 +2227,9 @@
       <c r="C112" t="n">
         <v>10</v>
       </c>
+      <c r="D112" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -1905,6 +2243,9 @@
       <c r="C113" t="n">
         <v>10</v>
       </c>
+      <c r="D113" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -1918,6 +2259,9 @@
       <c r="C114" t="n">
         <v>10</v>
       </c>
+      <c r="D114" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -1931,6 +2275,9 @@
       <c r="C115" t="n">
         <v>10</v>
       </c>
+      <c r="D115" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -1944,6 +2291,9 @@
       <c r="C116" t="n">
         <v>10</v>
       </c>
+      <c r="D116" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -1957,6 +2307,9 @@
       <c r="C117" t="n">
         <v>10</v>
       </c>
+      <c r="D117" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -1970,6 +2323,9 @@
       <c r="C118" t="n">
         <v>10</v>
       </c>
+      <c r="D118" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -1983,6 +2339,9 @@
       <c r="C119" t="n">
         <v>10</v>
       </c>
+      <c r="D119" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -1996,6 +2355,9 @@
       <c r="C120" t="n">
         <v>10</v>
       </c>
+      <c r="D120" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -2009,6 +2371,9 @@
       <c r="C121" t="n">
         <v>10</v>
       </c>
+      <c r="D121" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -2022,6 +2387,9 @@
       <c r="C122" t="n">
         <v>19</v>
       </c>
+      <c r="D122" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -2035,6 +2403,9 @@
       <c r="C123" t="n">
         <v>5</v>
       </c>
+      <c r="D123" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -2048,6 +2419,9 @@
       <c r="C124" t="n">
         <v>18</v>
       </c>
+      <c r="D124" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -2061,6 +2435,9 @@
       <c r="C125" t="n">
         <v>19</v>
       </c>
+      <c r="D125" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -2074,6 +2451,9 @@
       <c r="C126" t="n">
         <v>10</v>
       </c>
+      <c r="D126" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -2087,6 +2467,9 @@
       <c r="C127" t="n">
         <v>10</v>
       </c>
+      <c r="D127" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -2100,6 +2483,9 @@
       <c r="C128" t="n">
         <v>10</v>
       </c>
+      <c r="D128" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -2113,6 +2499,9 @@
       <c r="C129" t="n">
         <v>10</v>
       </c>
+      <c r="D129" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -2126,6 +2515,9 @@
       <c r="C130" t="n">
         <v>10</v>
       </c>
+      <c r="D130" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -2139,6 +2531,9 @@
       <c r="C131" t="n">
         <v>10</v>
       </c>
+      <c r="D131" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -2152,6 +2547,9 @@
       <c r="C132" t="n">
         <v>10</v>
       </c>
+      <c r="D132" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -2165,6 +2563,9 @@
       <c r="C133" t="n">
         <v>10</v>
       </c>
+      <c r="D133" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -2178,6 +2579,9 @@
       <c r="C134" t="n">
         <v>10</v>
       </c>
+      <c r="D134" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -2191,6 +2595,9 @@
       <c r="C135" t="n">
         <v>10</v>
       </c>
+      <c r="D135" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -2204,6 +2611,9 @@
       <c r="C136" t="n">
         <v>10</v>
       </c>
+      <c r="D136" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -2217,6 +2627,9 @@
       <c r="C137" t="n">
         <v>10</v>
       </c>
+      <c r="D137" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -2230,6 +2643,9 @@
       <c r="C138" t="n">
         <v>10</v>
       </c>
+      <c r="D138" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -2243,6 +2659,9 @@
       <c r="C139" t="n">
         <v>10</v>
       </c>
+      <c r="D139" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -2256,6 +2675,9 @@
       <c r="C140" t="n">
         <v>10</v>
       </c>
+      <c r="D140" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -2269,6 +2691,9 @@
       <c r="C141" t="n">
         <v>10</v>
       </c>
+      <c r="D141" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -2282,6 +2707,9 @@
       <c r="C142" t="n">
         <v>10</v>
       </c>
+      <c r="D142" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -2295,6 +2723,9 @@
       <c r="C143" t="n">
         <v>10</v>
       </c>
+      <c r="D143" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -2308,6 +2739,9 @@
       <c r="C144" t="n">
         <v>10</v>
       </c>
+      <c r="D144" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -2321,6 +2755,9 @@
       <c r="C145" t="n">
         <v>10</v>
       </c>
+      <c r="D145" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -2334,6 +2771,9 @@
       <c r="C146" t="n">
         <v>10</v>
       </c>
+      <c r="D146" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -2347,6 +2787,9 @@
       <c r="C147" t="n">
         <v>10</v>
       </c>
+      <c r="D147" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -2360,6 +2803,9 @@
       <c r="C148" t="n">
         <v>10</v>
       </c>
+      <c r="D148" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -2373,6 +2819,9 @@
       <c r="C149" t="n">
         <v>10</v>
       </c>
+      <c r="D149" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -2386,6 +2835,9 @@
       <c r="C150" t="n">
         <v>10</v>
       </c>
+      <c r="D150" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -2399,6 +2851,9 @@
       <c r="C151" t="n">
         <v>10</v>
       </c>
+      <c r="D151" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -2412,6 +2867,9 @@
       <c r="C152" t="n">
         <v>10</v>
       </c>
+      <c r="D152" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -2425,6 +2883,9 @@
       <c r="C153" t="n">
         <v>10</v>
       </c>
+      <c r="D153" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -2438,6 +2899,9 @@
       <c r="C154" t="n">
         <v>10</v>
       </c>
+      <c r="D154" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -2451,6 +2915,9 @@
       <c r="C155" t="n">
         <v>10</v>
       </c>
+      <c r="D155" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -2464,6 +2931,9 @@
       <c r="C156" t="n">
         <v>10</v>
       </c>
+      <c r="D156" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -2477,6 +2947,9 @@
       <c r="C157" t="n">
         <v>10</v>
       </c>
+      <c r="D157" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -2490,6 +2963,9 @@
       <c r="C158" t="n">
         <v>10</v>
       </c>
+      <c r="D158" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -2503,6 +2979,9 @@
       <c r="C159" t="n">
         <v>10</v>
       </c>
+      <c r="D159" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -2516,6 +2995,9 @@
       <c r="C160" t="n">
         <v>10</v>
       </c>
+      <c r="D160" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -2529,6 +3011,9 @@
       <c r="C161" t="n">
         <v>10</v>
       </c>
+      <c r="D161" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -2542,6 +3027,9 @@
       <c r="C162" t="n">
         <v>10</v>
       </c>
+      <c r="D162" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -2555,6 +3043,9 @@
       <c r="C163" t="n">
         <v>10</v>
       </c>
+      <c r="D163" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -2568,6 +3059,9 @@
       <c r="C164" t="n">
         <v>10</v>
       </c>
+      <c r="D164" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -2581,6 +3075,9 @@
       <c r="C165" t="n">
         <v>10</v>
       </c>
+      <c r="D165" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -2594,6 +3091,9 @@
       <c r="C166" t="n">
         <v>10</v>
       </c>
+      <c r="D166" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -2607,6 +3107,9 @@
       <c r="C167" t="n">
         <v>9</v>
       </c>
+      <c r="D167" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -2620,6 +3123,9 @@
       <c r="C168" t="n">
         <v>10</v>
       </c>
+      <c r="D168" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -2633,6 +3139,9 @@
       <c r="C169" t="n">
         <v>11</v>
       </c>
+      <c r="D169" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -2646,6 +3155,9 @@
       <c r="C170" t="n">
         <v>10</v>
       </c>
+      <c r="D170" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
@@ -2659,6 +3171,9 @@
       <c r="C171" t="n">
         <v>10</v>
       </c>
+      <c r="D171" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -2672,6 +3187,9 @@
       <c r="C172" t="n">
         <v>10</v>
       </c>
+      <c r="D172" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -2685,6 +3203,9 @@
       <c r="C173" t="n">
         <v>10</v>
       </c>
+      <c r="D173" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -2698,6 +3219,9 @@
       <c r="C174" t="n">
         <v>10</v>
       </c>
+      <c r="D174" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -2711,6 +3235,9 @@
       <c r="C175" t="n">
         <v>10</v>
       </c>
+      <c r="D175" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -2724,6 +3251,9 @@
       <c r="C176" t="n">
         <v>10</v>
       </c>
+      <c r="D176" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -2737,6 +3267,9 @@
       <c r="C177" t="n">
         <v>10</v>
       </c>
+      <c r="D177" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -2750,6 +3283,9 @@
       <c r="C178" t="n">
         <v>10</v>
       </c>
+      <c r="D178" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
@@ -2763,6 +3299,9 @@
       <c r="C179" t="n">
         <v>10</v>
       </c>
+      <c r="D179" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -2776,6 +3315,9 @@
       <c r="C180" t="n">
         <v>10</v>
       </c>
+      <c r="D180" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -2789,6 +3331,9 @@
       <c r="C181" t="n">
         <v>10</v>
       </c>
+      <c r="D181" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
@@ -2802,6 +3347,9 @@
       <c r="C182" t="n">
         <v>10</v>
       </c>
+      <c r="D182" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -2815,6 +3363,9 @@
       <c r="C183" t="n">
         <v>10</v>
       </c>
+      <c r="D183" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -2828,6 +3379,9 @@
       <c r="C184" t="n">
         <v>10</v>
       </c>
+      <c r="D184" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -2841,6 +3395,9 @@
       <c r="C185" t="n">
         <v>10</v>
       </c>
+      <c r="D185" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -2854,6 +3411,9 @@
       <c r="C186" t="n">
         <v>10</v>
       </c>
+      <c r="D186" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -2867,6 +3427,9 @@
       <c r="C187" t="n">
         <v>10</v>
       </c>
+      <c r="D187" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
@@ -2880,6 +3443,9 @@
       <c r="C188" t="n">
         <v>10</v>
       </c>
+      <c r="D188" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -2893,6 +3459,9 @@
       <c r="C189" t="n">
         <v>10</v>
       </c>
+      <c r="D189" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
@@ -2906,6 +3475,9 @@
       <c r="C190" t="n">
         <v>10</v>
       </c>
+      <c r="D190" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
@@ -2919,6 +3491,9 @@
       <c r="C191" t="n">
         <v>10</v>
       </c>
+      <c r="D191" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -2932,6 +3507,9 @@
       <c r="C192" t="n">
         <v>10</v>
       </c>
+      <c r="D192" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -2945,6 +3523,9 @@
       <c r="C193" t="n">
         <v>10</v>
       </c>
+      <c r="D193" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -2958,6 +3539,9 @@
       <c r="C194" t="n">
         <v>10</v>
       </c>
+      <c r="D194" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
@@ -2971,6 +3555,9 @@
       <c r="C195" t="n">
         <v>10</v>
       </c>
+      <c r="D195" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
@@ -2984,6 +3571,9 @@
       <c r="C196" t="n">
         <v>11</v>
       </c>
+      <c r="D196" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
@@ -2997,6 +3587,9 @@
       <c r="C197" t="n">
         <v>10</v>
       </c>
+      <c r="D197" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -3010,6 +3603,9 @@
       <c r="C198" t="n">
         <v>9</v>
       </c>
+      <c r="D198" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -3023,6 +3619,9 @@
       <c r="C199" t="n">
         <v>10</v>
       </c>
+      <c r="D199" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -3036,6 +3635,9 @@
       <c r="C200" t="n">
         <v>10</v>
       </c>
+      <c r="D200" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
@@ -3049,6 +3651,9 @@
       <c r="C201" t="n">
         <v>10</v>
       </c>
+      <c r="D201" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
@@ -3062,6 +3667,9 @@
       <c r="C202" t="n">
         <v>10</v>
       </c>
+      <c r="D202" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -3075,6 +3683,9 @@
       <c r="C203" t="n">
         <v>10</v>
       </c>
+      <c r="D203" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
@@ -3088,6 +3699,9 @@
       <c r="C204" t="n">
         <v>10</v>
       </c>
+      <c r="D204" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
@@ -3101,6 +3715,9 @@
       <c r="C205" t="n">
         <v>10</v>
       </c>
+      <c r="D205" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
@@ -3114,6 +3731,9 @@
       <c r="C206" t="n">
         <v>10</v>
       </c>
+      <c r="D206" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -3127,6 +3747,9 @@
       <c r="C207" t="n">
         <v>10</v>
       </c>
+      <c r="D207" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
@@ -3140,6 +3763,9 @@
       <c r="C208" t="n">
         <v>10</v>
       </c>
+      <c r="D208" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
@@ -3153,6 +3779,9 @@
       <c r="C209" t="n">
         <v>10</v>
       </c>
+      <c r="D209" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
@@ -3166,6 +3795,9 @@
       <c r="C210" t="n">
         <v>10</v>
       </c>
+      <c r="D210" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
@@ -3179,6 +3811,9 @@
       <c r="C211" t="n">
         <v>10</v>
       </c>
+      <c r="D211" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
@@ -3192,6 +3827,9 @@
       <c r="C212" t="n">
         <v>10</v>
       </c>
+      <c r="D212" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
@@ -3205,6 +3843,9 @@
       <c r="C213" t="n">
         <v>10</v>
       </c>
+      <c r="D213" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
@@ -3218,6 +3859,9 @@
       <c r="C214" t="n">
         <v>10</v>
       </c>
+      <c r="D214" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
@@ -3231,6 +3875,9 @@
       <c r="C215" t="n">
         <v>10</v>
       </c>
+      <c r="D215" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
@@ -3244,6 +3891,9 @@
       <c r="C216" t="n">
         <v>10</v>
       </c>
+      <c r="D216" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
@@ -3257,6 +3907,9 @@
       <c r="C217" t="n">
         <v>10</v>
       </c>
+      <c r="D217" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
@@ -3270,6 +3923,9 @@
       <c r="C218" t="n">
         <v>11</v>
       </c>
+      <c r="D218" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -3283,6 +3939,9 @@
       <c r="C219" t="n">
         <v>10</v>
       </c>
+      <c r="D219" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
@@ -3296,6 +3955,9 @@
       <c r="C220" t="n">
         <v>10</v>
       </c>
+      <c r="D220" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
@@ -3309,6 +3971,9 @@
       <c r="C221" t="n">
         <v>10</v>
       </c>
+      <c r="D221" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -3322,6 +3987,9 @@
       <c r="C222" t="n">
         <v>10</v>
       </c>
+      <c r="D222" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -3335,6 +4003,9 @@
       <c r="C223" t="n">
         <v>9</v>
       </c>
+      <c r="D223" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -3348,6 +4019,9 @@
       <c r="C224" t="n">
         <v>10</v>
       </c>
+      <c r="D224" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
@@ -3361,6 +4035,9 @@
       <c r="C225" t="n">
         <v>10</v>
       </c>
+      <c r="D225" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
@@ -3374,6 +4051,9 @@
       <c r="C226" t="n">
         <v>10</v>
       </c>
+      <c r="D226" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -3387,6 +4067,9 @@
       <c r="C227" t="n">
         <v>10</v>
       </c>
+      <c r="D227" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
@@ -3400,6 +4083,9 @@
       <c r="C228" t="n">
         <v>10</v>
       </c>
+      <c r="D228" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -3413,6 +4099,9 @@
       <c r="C229" t="n">
         <v>10</v>
       </c>
+      <c r="D229" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
@@ -3426,6 +4115,9 @@
       <c r="C230" t="n">
         <v>10</v>
       </c>
+      <c r="D230" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
@@ -3439,6 +4131,9 @@
       <c r="C231" t="n">
         <v>10</v>
       </c>
+      <c r="D231" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
@@ -3452,6 +4147,9 @@
       <c r="C232" t="n">
         <v>10</v>
       </c>
+      <c r="D232" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -3465,6 +4163,9 @@
       <c r="C233" t="n">
         <v>10</v>
       </c>
+      <c r="D233" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -3478,6 +4179,9 @@
       <c r="C234" t="n">
         <v>10</v>
       </c>
+      <c r="D234" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
@@ -3491,6 +4195,9 @@
       <c r="C235" t="n">
         <v>9</v>
       </c>
+      <c r="D235" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
@@ -3504,6 +4211,9 @@
       <c r="C236" t="n">
         <v>10</v>
       </c>
+      <c r="D236" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
@@ -3517,6 +4227,9 @@
       <c r="C237" t="n">
         <v>10</v>
       </c>
+      <c r="D237" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
@@ -3530,6 +4243,9 @@
       <c r="C238" t="n">
         <v>10</v>
       </c>
+      <c r="D238" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
@@ -3543,6 +4259,9 @@
       <c r="C239" t="n">
         <v>10</v>
       </c>
+      <c r="D239" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -3556,6 +4275,9 @@
       <c r="C240" t="n">
         <v>10</v>
       </c>
+      <c r="D240" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
@@ -3569,6 +4291,9 @@
       <c r="C241" t="n">
         <v>10</v>
       </c>
+      <c r="D241" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
@@ -3582,6 +4307,9 @@
       <c r="C242" t="n">
         <v>10</v>
       </c>
+      <c r="D242" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
@@ -3595,6 +4323,9 @@
       <c r="C243" t="n">
         <v>10</v>
       </c>
+      <c r="D243" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
@@ -3608,6 +4339,9 @@
       <c r="C244" t="n">
         <v>10</v>
       </c>
+      <c r="D244" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
@@ -3621,6 +4355,9 @@
       <c r="C245" t="n">
         <v>10</v>
       </c>
+      <c r="D245" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
@@ -3634,6 +4371,9 @@
       <c r="C246" t="n">
         <v>10</v>
       </c>
+      <c r="D246" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
@@ -3647,6 +4387,9 @@
       <c r="C247" t="n">
         <v>10</v>
       </c>
+      <c r="D247" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
@@ -3660,6 +4403,9 @@
       <c r="C248" t="n">
         <v>10</v>
       </c>
+      <c r="D248" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
@@ -3673,6 +4419,9 @@
       <c r="C249" t="n">
         <v>10</v>
       </c>
+      <c r="D249" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
@@ -3686,6 +4435,9 @@
       <c r="C250" t="n">
         <v>10</v>
       </c>
+      <c r="D250" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
@@ -3699,6 +4451,9 @@
       <c r="C251" t="n">
         <v>10</v>
       </c>
+      <c r="D251" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
@@ -3712,6 +4467,9 @@
       <c r="C252" t="n">
         <v>10</v>
       </c>
+      <c r="D252" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
@@ -3725,6 +4483,9 @@
       <c r="C253" t="n">
         <v>10</v>
       </c>
+      <c r="D253" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
@@ -3738,6 +4499,9 @@
       <c r="C254" t="n">
         <v>10</v>
       </c>
+      <c r="D254" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
@@ -3751,6 +4515,9 @@
       <c r="C255" t="n">
         <v>10</v>
       </c>
+      <c r="D255" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
@@ -3764,6 +4531,9 @@
       <c r="C256" t="n">
         <v>10</v>
       </c>
+      <c r="D256" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
@@ -3777,6 +4547,9 @@
       <c r="C257" t="n">
         <v>10</v>
       </c>
+      <c r="D257" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
@@ -3790,6 +4563,9 @@
       <c r="C258" t="n">
         <v>10</v>
       </c>
+      <c r="D258" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
@@ -3803,6 +4579,9 @@
       <c r="C259" t="n">
         <v>10</v>
       </c>
+      <c r="D259" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
@@ -3816,6 +4595,9 @@
       <c r="C260" t="n">
         <v>10</v>
       </c>
+      <c r="D260" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
@@ -3829,6 +4611,9 @@
       <c r="C261" t="n">
         <v>10</v>
       </c>
+      <c r="D261" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
@@ -3842,6 +4627,9 @@
       <c r="C262" t="n">
         <v>10</v>
       </c>
+      <c r="D262" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
@@ -3855,6 +4643,9 @@
       <c r="C263" t="n">
         <v>10</v>
       </c>
+      <c r="D263" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
@@ -3868,6 +4659,9 @@
       <c r="C264" t="n">
         <v>10</v>
       </c>
+      <c r="D264" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
@@ -3881,6 +4675,9 @@
       <c r="C265" t="n">
         <v>10</v>
       </c>
+      <c r="D265" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
@@ -3894,6 +4691,9 @@
       <c r="C266" t="n">
         <v>10</v>
       </c>
+      <c r="D266" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
@@ -3907,6 +4707,9 @@
       <c r="C267" t="n">
         <v>10</v>
       </c>
+      <c r="D267" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
@@ -3920,6 +4723,9 @@
       <c r="C268" t="n">
         <v>10</v>
       </c>
+      <c r="D268" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
@@ -3933,6 +4739,9 @@
       <c r="C269" t="n">
         <v>10</v>
       </c>
+      <c r="D269" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
@@ -3946,6 +4755,9 @@
       <c r="C270" t="n">
         <v>10</v>
       </c>
+      <c r="D270" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
@@ -3959,6 +4771,9 @@
       <c r="C271" t="n">
         <v>10</v>
       </c>
+      <c r="D271" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
@@ -3972,6 +4787,9 @@
       <c r="C272" t="n">
         <v>10</v>
       </c>
+      <c r="D272" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
@@ -3985,6 +4803,9 @@
       <c r="C273" t="n">
         <v>10</v>
       </c>
+      <c r="D273" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
@@ -3998,6 +4819,9 @@
       <c r="C274" t="n">
         <v>10</v>
       </c>
+      <c r="D274" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
@@ -4011,6 +4835,9 @@
       <c r="C275" t="n">
         <v>10</v>
       </c>
+      <c r="D275" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
@@ -4024,6 +4851,9 @@
       <c r="C276" t="n">
         <v>10</v>
       </c>
+      <c r="D276" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
@@ -4037,6 +4867,9 @@
       <c r="C277" t="n">
         <v>10</v>
       </c>
+      <c r="D277" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
@@ -4050,6 +4883,9 @@
       <c r="C278" t="n">
         <v>10</v>
       </c>
+      <c r="D278" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
@@ -4063,6 +4899,9 @@
       <c r="C279" t="n">
         <v>11</v>
       </c>
+      <c r="D279" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
@@ -4076,6 +4915,9 @@
       <c r="C280" t="n">
         <v>10</v>
       </c>
+      <c r="D280" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
@@ -4089,6 +4931,9 @@
       <c r="C281" t="n">
         <v>10</v>
       </c>
+      <c r="D281" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -4102,6 +4947,9 @@
       <c r="C282" t="n">
         <v>11</v>
       </c>
+      <c r="D282" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
@@ -4115,6 +4963,9 @@
       <c r="C283" t="n">
         <v>10</v>
       </c>
+      <c r="D283" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -4128,6 +4979,9 @@
       <c r="C284" t="n">
         <v>10</v>
       </c>
+      <c r="D284" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
@@ -4141,6 +4995,9 @@
       <c r="C285" t="n">
         <v>10</v>
       </c>
+      <c r="D285" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
@@ -4154,6 +5011,9 @@
       <c r="C286" t="n">
         <v>10</v>
       </c>
+      <c r="D286" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
@@ -4167,6 +5027,9 @@
       <c r="C287" t="n">
         <v>10</v>
       </c>
+      <c r="D287" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
@@ -4180,6 +5043,9 @@
       <c r="C288" t="n">
         <v>10</v>
       </c>
+      <c r="D288" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -4193,6 +5059,9 @@
       <c r="C289" t="n">
         <v>10</v>
       </c>
+      <c r="D289" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
@@ -4206,6 +5075,9 @@
       <c r="C290" t="n">
         <v>10</v>
       </c>
+      <c r="D290" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
@@ -4219,6 +5091,9 @@
       <c r="C291" t="n">
         <v>10</v>
       </c>
+      <c r="D291" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
@@ -4232,6 +5107,9 @@
       <c r="C292" t="n">
         <v>10</v>
       </c>
+      <c r="D292" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
@@ -4245,6 +5123,9 @@
       <c r="C293" t="n">
         <v>10</v>
       </c>
+      <c r="D293" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
@@ -4258,6 +5139,9 @@
       <c r="C294" t="n">
         <v>10</v>
       </c>
+      <c r="D294" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
@@ -4271,6 +5155,9 @@
       <c r="C295" t="n">
         <v>10</v>
       </c>
+      <c r="D295" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
@@ -4284,6 +5171,9 @@
       <c r="C296" t="n">
         <v>10</v>
       </c>
+      <c r="D296" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
@@ -4297,6 +5187,9 @@
       <c r="C297" t="n">
         <v>10</v>
       </c>
+      <c r="D297" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
@@ -4310,6 +5203,9 @@
       <c r="C298" t="n">
         <v>10</v>
       </c>
+      <c r="D298" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
@@ -4323,6 +5219,9 @@
       <c r="C299" t="n">
         <v>10</v>
       </c>
+      <c r="D299" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
@@ -4336,6 +5235,9 @@
       <c r="C300" t="n">
         <v>9</v>
       </c>
+      <c r="D300" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
@@ -4349,6 +5251,9 @@
       <c r="C301" t="n">
         <v>10</v>
       </c>
+      <c r="D301" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
@@ -4362,6 +5267,9 @@
       <c r="C302" t="n">
         <v>10</v>
       </c>
+      <c r="D302" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
@@ -4375,6 +5283,9 @@
       <c r="C303" t="n">
         <v>10</v>
       </c>
+      <c r="D303" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
@@ -4388,6 +5299,9 @@
       <c r="C304" t="n">
         <v>10</v>
       </c>
+      <c r="D304" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
@@ -4401,6 +5315,9 @@
       <c r="C305" t="n">
         <v>10</v>
       </c>
+      <c r="D305" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
@@ -4414,6 +5331,9 @@
       <c r="C306" t="n">
         <v>10</v>
       </c>
+      <c r="D306" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
@@ -4427,6 +5347,9 @@
       <c r="C307" t="n">
         <v>10</v>
       </c>
+      <c r="D307" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
@@ -4440,6 +5363,9 @@
       <c r="C308" t="n">
         <v>10</v>
       </c>
+      <c r="D308" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
@@ -4453,6 +5379,9 @@
       <c r="C309" t="n">
         <v>10</v>
       </c>
+      <c r="D309" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
@@ -4466,6 +5395,9 @@
       <c r="C310" t="n">
         <v>10</v>
       </c>
+      <c r="D310" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
@@ -4479,6 +5411,9 @@
       <c r="C311" t="n">
         <v>10</v>
       </c>
+      <c r="D311" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
@@ -4492,6 +5427,9 @@
       <c r="C312" t="n">
         <v>10</v>
       </c>
+      <c r="D312" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
@@ -4505,6 +5443,9 @@
       <c r="C313" t="n">
         <v>10</v>
       </c>
+      <c r="D313" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
@@ -4518,6 +5459,9 @@
       <c r="C314" t="n">
         <v>10</v>
       </c>
+      <c r="D314" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
@@ -4531,6 +5475,9 @@
       <c r="C315" t="n">
         <v>10</v>
       </c>
+      <c r="D315" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
@@ -4544,6 +5491,9 @@
       <c r="C316" t="n">
         <v>10</v>
       </c>
+      <c r="D316" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
@@ -4557,6 +5507,9 @@
       <c r="C317" t="n">
         <v>10</v>
       </c>
+      <c r="D317" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
@@ -4570,6 +5523,9 @@
       <c r="C318" t="n">
         <v>9</v>
       </c>
+      <c r="D318" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
@@ -4583,6 +5539,9 @@
       <c r="C319" t="n">
         <v>10</v>
       </c>
+      <c r="D319" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
@@ -4596,6 +5555,9 @@
       <c r="C320" t="n">
         <v>10</v>
       </c>
+      <c r="D320" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
@@ -4609,6 +5571,9 @@
       <c r="C321" t="n">
         <v>10</v>
       </c>
+      <c r="D321" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
@@ -4622,6 +5587,9 @@
       <c r="C322" t="n">
         <v>10</v>
       </c>
+      <c r="D322" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
@@ -4635,6 +5603,9 @@
       <c r="C323" t="n">
         <v>10</v>
       </c>
+      <c r="D323" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
@@ -4648,6 +5619,9 @@
       <c r="C324" t="n">
         <v>10</v>
       </c>
+      <c r="D324" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
@@ -4661,6 +5635,9 @@
       <c r="C325" t="n">
         <v>10</v>
       </c>
+      <c r="D325" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
@@ -4674,6 +5651,9 @@
       <c r="C326" t="n">
         <v>10</v>
       </c>
+      <c r="D326" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
@@ -4687,6 +5667,9 @@
       <c r="C327" t="n">
         <v>10</v>
       </c>
+      <c r="D327" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
@@ -4700,6 +5683,9 @@
       <c r="C328" t="n">
         <v>10</v>
       </c>
+      <c r="D328" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
@@ -4713,6 +5699,9 @@
       <c r="C329" t="n">
         <v>10</v>
       </c>
+      <c r="D329" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
@@ -4726,6 +5715,9 @@
       <c r="C330" t="n">
         <v>10</v>
       </c>
+      <c r="D330" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
@@ -4739,6 +5731,9 @@
       <c r="C331" t="n">
         <v>9</v>
       </c>
+      <c r="D331" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
@@ -4752,6 +5747,9 @@
       <c r="C332" t="n">
         <v>10</v>
       </c>
+      <c r="D332" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
@@ -4765,6 +5763,9 @@
       <c r="C333" t="n">
         <v>10</v>
       </c>
+      <c r="D333" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
@@ -4778,6 +5779,9 @@
       <c r="C334" t="n">
         <v>10</v>
       </c>
+      <c r="D334" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
@@ -4791,6 +5795,9 @@
       <c r="C335" t="n">
         <v>10</v>
       </c>
+      <c r="D335" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
@@ -4804,6 +5811,9 @@
       <c r="C336" t="n">
         <v>10</v>
       </c>
+      <c r="D336" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
@@ -4817,6 +5827,9 @@
       <c r="C337" t="n">
         <v>10</v>
       </c>
+      <c r="D337" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
@@ -4830,6 +5843,9 @@
       <c r="C338" t="n">
         <v>10</v>
       </c>
+      <c r="D338" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
@@ -4843,6 +5859,9 @@
       <c r="C339" t="n">
         <v>10</v>
       </c>
+      <c r="D339" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
@@ -4856,6 +5875,9 @@
       <c r="C340" t="n">
         <v>10</v>
       </c>
+      <c r="D340" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
@@ -4869,6 +5891,9 @@
       <c r="C341" t="n">
         <v>10</v>
       </c>
+      <c r="D341" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
@@ -4882,6 +5907,9 @@
       <c r="C342" t="n">
         <v>10</v>
       </c>
+      <c r="D342" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
@@ -4895,6 +5923,9 @@
       <c r="C343" t="n">
         <v>10</v>
       </c>
+      <c r="D343" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
@@ -4908,6 +5939,9 @@
       <c r="C344" t="n">
         <v>10</v>
       </c>
+      <c r="D344" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
@@ -4919,6 +5953,9 @@
         </is>
       </c>
       <c r="C345" t="n">
+        <v>10</v>
+      </c>
+      <c r="D345" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>